<commit_message>
fix variable shape import
</commit_message>
<xml_diff>
--- a/test/fixtures/excel_mda_sample.xlsx
+++ b/test/fixtures/excel_mda_sample.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="230">
   <si>
     <t>N</t>
   </si>
@@ -697,9 +697,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>X3</t>
-  </si>
-  <si>
     <t>X2</t>
   </si>
   <si>
@@ -718,7 +715,7 @@
     <t>Y2</t>
   </si>
   <si>
-    <t>(2, )</t>
+    <t>(2,)</t>
   </si>
 </sst>
 </file>
@@ -1203,6 +1200,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1227,10 +1228,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -2206,8 +2203,8 @@
   </sheetPr>
   <dimension ref="B1:P58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2332,14 +2329,14 @@
       <c r="P6"/>
     </row>
     <row r="7" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="E7" s="37" t="s">
+      <c r="C7" s="40"/>
+      <c r="E7" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="38"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
@@ -2436,23 +2433,23 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="43"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
@@ -2469,7 +2466,7 @@
         <v>214</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="27" t="s">
@@ -2514,7 +2511,7 @@
         <v>9</v>
       </c>
       <c r="K16" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
@@ -2544,10 +2541,10 @@
         <v>15</v>
       </c>
       <c r="J17" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="K17" s="27" t="s">
         <v>225</v>
-      </c>
-      <c r="K17" s="27" t="s">
-        <v>226</v>
       </c>
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
@@ -2577,10 +2574,10 @@
         <v>15</v>
       </c>
       <c r="J18" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="K18" s="27" t="s">
         <v>227</v>
-      </c>
-      <c r="K18" s="27" t="s">
-        <v>228</v>
       </c>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
@@ -2610,7 +2607,7 @@
         <v>15</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
@@ -2641,7 +2638,7 @@
         <v>15</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
@@ -2651,7 +2648,7 @@
       <c r="P20" s="28"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="26" t="s">
@@ -2672,33 +2669,33 @@
         <v>15</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
       <c r="N21" s="27"/>
       <c r="O21" s="27"/>
-      <c r="P21" s="46"/>
+      <c r="P21" s="38"/>
     </row>
     <row r="22" spans="2:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="46"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F23" s="2"/>
@@ -2794,7 +2791,7 @@
     <row r="52" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="6:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>